<commit_message>
more ded added sample
</commit_message>
<xml_diff>
--- a/ptsdoctor.xlsx
+++ b/ptsdoctor.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="30">
   <si>
     <t xml:space="preserve">Disease_id</t>
   </si>
@@ -57,15 +57,21 @@
     <t xml:space="preserve">nil</t>
   </si>
   <si>
+    <t xml:space="preserve">abc,mno</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cba</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/seenuvasan1947/ptsdoctor-data/raw/main/healthy.txt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">abc,bnm</t>
+  </si>
+  <si>
     <t xml:space="preserve">abc</t>
   </si>
   <si>
-    <t xml:space="preserve">cba</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://github.com/seenuvasan1947/ptsdoctor-data/raw/main/healthy.txt</t>
-  </si>
-  <si>
     <t xml:space="preserve">Io_medicine_name</t>
   </si>
   <si>
@@ -88,6 +94,12 @@
   </si>
   <si>
     <t xml:space="preserve">sugar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mno</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bnm</t>
   </si>
   <si>
     <t xml:space="preserve">O_medicine_name</t>
@@ -109,7 +121,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -138,12 +150,6 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF0000FF"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -200,7 +206,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -223,11 +229,11 @@
   </sheetPr>
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="86" zoomScaleNormal="86" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="86" zoomScaleNormal="86" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.44"/>
@@ -304,7 +310,7 @@
         <v>10</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="F3" s="0" t="s">
         <v>12</v>
@@ -330,7 +336,7 @@
         <v>10</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="F4" s="0" t="s">
         <v>12</v>
@@ -356,7 +362,7 @@
         <v>10</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="F5" s="0" t="s">
         <v>12</v>
@@ -382,7 +388,7 @@
         <v>10</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="F6" s="0" t="s">
         <v>12</v>
@@ -417,13 +423,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="86" zoomScaleNormal="86" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="86" zoomScaleNormal="86" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.2"/>
@@ -435,30 +441,30 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C1" s="0" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>1</v>
@@ -467,15 +473,57 @@
         <v>13</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F2" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="0" t="s">
         <v>21</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" display="https://github.com/seenuvasan1947/ptsdoctor-data/raw/main/healthy.txt"/>
+    <hyperlink ref="D3" r:id="rId2" display="https://github.com/seenuvasan1947/ptsdoctor-data/raw/main/healthy.txt"/>
+    <hyperlink ref="D4" r:id="rId3" display="https://github.com/seenuvasan1947/ptsdoctor-data/raw/main/healthy.txt"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -498,7 +546,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.2"/>
@@ -510,22 +558,22 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C1" s="0" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -533,7 +581,7 @@
         <v>12</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>1</v>
@@ -542,10 +590,10 @@
         <v>13</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>